<commit_message>
metodologia p seleccion socios
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/Datos/Construcción socios comerciales/socios_expo.xlsx
+++ b/Archivos de trabajo/Datos/Construcción socios comerciales/socios_expo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd03ae9016654ccc/Escritorio/Paper-ITCRM.SF/Archivos de trabajo/Datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd03ae9016654ccc/Escritorio/Paper-ITCRM.SF/Archivos de trabajo/Datos/Construcción socios comerciales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{AEFDB262-F85A-4503-9F9C-FB96FD9C40B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C97CD1A-4E82-4E3D-972A-B43E0EE19AB2}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{AEFDB262-F85A-4503-9F9C-FB96FD9C40B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7A01CF7-CBF8-4C60-B288-0EEEA421AD00}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="top fob" sheetId="7" r:id="rId1"/>
@@ -859,7 +859,9 @@
   </sheetPr>
   <dimension ref="A1:HR30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7391,7 +7393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9886,10 +9888,10 @@
   <dimension ref="A1:AG52"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10003,7 +10005,7 @@
         <v>39</v>
       </c>
       <c r="C2" s="7">
-        <f t="shared" ref="C2:C25" si="0">SUM(D2:AF2)</f>
+        <f>SUM(D2:AF2)</f>
         <v>0.77087622753295992</v>
       </c>
       <c r="D2" s="4">
@@ -10131,7 +10133,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C2:C25" si="0">SUM(D3:AF3)</f>
         <v>0.78334929518237717</v>
       </c>
       <c r="D3" s="4">

</xml_diff>